<commit_message>
Tester Suresh commited 04-15-2019
</commit_message>
<xml_diff>
--- a/Excel_Sheet/SmokeTestCaseHireMee.xlsx
+++ b/Excel_Sheet/SmokeTestCaseHireMee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="7" tabRatio="812" windowHeight="11130" windowWidth="23085" xWindow="0" yWindow="2505"/>
+    <workbookView activeTab="1" tabRatio="812" windowHeight="11130" windowWidth="23085" xWindow="0" yWindow="2505"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" r:id="rId1" sheetId="5"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2678" uniqueCount="740">
   <si>
     <t>Project Name</t>
   </si>
@@ -4776,8 +4776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N218"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5769,7 +5769,7 @@
       </c>
       <c r="K38" s="14"/>
       <c r="L38" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row ht="31.5" r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -7586,7 +7586,7 @@
         <v>737</v>
       </c>
       <c r="L21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="60" r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -7624,7 +7624,7 @@
         <v>375</v>
       </c>
       <c r="L22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row customHeight="1" ht="50.25" r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -11421,8 +11421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CS59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13626,7 +13626,7 @@
         <v>739</v>
       </c>
       <c r="L20" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row ht="75" r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -14314,7 +14314,7 @@
       </c>
       <c r="K39" s="103"/>
       <c r="L39" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automation tester suresh commmited
</commit_message>
<xml_diff>
--- a/Excel_Sheet/SmokeTestCaseHireMee.xlsx
+++ b/Excel_Sheet/SmokeTestCaseHireMee.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2678" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3142" uniqueCount="740">
   <si>
     <t>Project Name</t>
   </si>
@@ -5116,7 +5116,7 @@
         <v>735</v>
       </c>
       <c r="L20" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M20" s="18"/>
     </row>
@@ -5769,7 +5769,7 @@
       </c>
       <c r="K38" s="14"/>
       <c r="L38" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="31.5" r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -7586,7 +7586,7 @@
         <v>737</v>
       </c>
       <c r="L21" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row ht="60" r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -7624,7 +7624,7 @@
         <v>375</v>
       </c>
       <c r="L22" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row customHeight="1" ht="50.25" r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -14314,7 +14314,7 @@
       </c>
       <c r="K39" s="103"/>
       <c r="L39" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suresh commited on 05/15/2019
</commit_message>
<xml_diff>
--- a/Excel_Sheet/SmokeTestCaseHireMee.xlsx
+++ b/Excel_Sheet/SmokeTestCaseHireMee.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3142" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="740">
   <si>
     <t>Project Name</t>
   </si>
@@ -5116,7 +5116,7 @@
         <v>735</v>
       </c>
       <c r="L20" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="M20" s="18"/>
     </row>
@@ -6783,7 +6783,7 @@
         <v>734</v>
       </c>
       <c r="L21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="75" r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -6821,7 +6821,7 @@
         <v>375</v>
       </c>
       <c r="L22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -6857,7 +6857,7 @@
       </c>
       <c r="K23" s="25"/>
       <c r="L23" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -7109,7 +7109,7 @@
       </c>
       <c r="K30" s="25"/>
       <c r="L30" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -7586,7 +7586,7 @@
         <v>737</v>
       </c>
       <c r="L21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="60" r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -7624,7 +7624,7 @@
         <v>375</v>
       </c>
       <c r="L22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row customHeight="1" ht="50.25" r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -8749,7 +8749,7 @@
         <v>736</v>
       </c>
       <c r="L20" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
@@ -8885,7 +8885,7 @@
         <v>738</v>
       </c>
       <c r="L21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="75" r="22" spans="1:110" x14ac:dyDescent="0.25">
@@ -8923,7 +8923,7 @@
         <v>375</v>
       </c>
       <c r="L22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="30" r="23" spans="1:110" x14ac:dyDescent="0.25">
@@ -11139,7 +11139,7 @@
         <v>731</v>
       </c>
       <c r="L20" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
@@ -11205,7 +11205,7 @@
       </c>
       <c r="K21" s="78"/>
       <c r="L21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="60" r="22" spans="1:42" x14ac:dyDescent="0.25">
@@ -11241,7 +11241,7 @@
       </c>
       <c r="K22" s="79"/>
       <c r="L22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="60" r="23" spans="1:42" x14ac:dyDescent="0.25">
@@ -11277,7 +11277,7 @@
       </c>
       <c r="K23" s="30"/>
       <c r="L23" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="60" r="24" spans="1:42" x14ac:dyDescent="0.25">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="K24" s="14"/>
       <c r="L24" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="60" r="25" spans="1:42" x14ac:dyDescent="0.25">
@@ -11349,7 +11349,7 @@
       </c>
       <c r="K25" s="14"/>
       <c r="L25" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="15.75" r="27" spans="1:42" x14ac:dyDescent="0.25">
@@ -11754,7 +11754,7 @@
         <v>731</v>
       </c>
       <c r="L20" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M20" s="82"/>
       <c r="N20" s="82"/>
@@ -11874,7 +11874,7 @@
       </c>
       <c r="K21" s="54"/>
       <c r="L21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M21" s="82"/>
       <c r="N21" s="82"/>
@@ -11994,7 +11994,7 @@
       </c>
       <c r="K22" s="54"/>
       <c r="L22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row customFormat="1" ht="60" r="23" s="82" spans="1:96" x14ac:dyDescent="0.25">
@@ -12030,7 +12030,7 @@
       </c>
       <c r="K23" s="54"/>
       <c r="L23" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row customFormat="1" ht="60" r="24" s="82" spans="1:96" x14ac:dyDescent="0.25">
@@ -12066,7 +12066,7 @@
       </c>
       <c r="K24" s="54"/>
       <c r="L24" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row customFormat="1" ht="75" r="25" s="82" spans="1:96" x14ac:dyDescent="0.25">
@@ -12098,7 +12098,7 @@
       <c r="J25" s="14"/>
       <c r="K25" s="54"/>
       <c r="L25" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row customFormat="1" ht="45" r="26" s="82" spans="1:96" x14ac:dyDescent="0.25">
@@ -12134,7 +12134,7 @@
       </c>
       <c r="K26" s="81"/>
       <c r="L26" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
@@ -12884,7 +12884,7 @@
       </c>
       <c r="K46" s="84"/>
       <c r="L46" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -12920,7 +12920,7 @@
       </c>
       <c r="K47" s="84"/>
       <c r="L47" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -12956,7 +12956,7 @@
       </c>
       <c r="K48" s="84"/>
       <c r="L48" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -12992,7 +12992,7 @@
       </c>
       <c r="K49" s="84"/>
       <c r="L49" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -13028,7 +13028,7 @@
       </c>
       <c r="K50" s="84"/>
       <c r="L50" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -13064,7 +13064,7 @@
       </c>
       <c r="K51" s="84"/>
       <c r="L51" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -13100,7 +13100,7 @@
       </c>
       <c r="K52" s="84"/>
       <c r="L52" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -13136,7 +13136,7 @@
       </c>
       <c r="K53" s="84"/>
       <c r="L53" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -13172,7 +13172,7 @@
       </c>
       <c r="K54" s="84"/>
       <c r="L54" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -13208,7 +13208,7 @@
       </c>
       <c r="K55" s="84"/>
       <c r="L55" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -13244,7 +13244,7 @@
       </c>
       <c r="K56" s="84"/>
       <c r="L56" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -13280,7 +13280,7 @@
       </c>
       <c r="K57" s="84"/>
       <c r="L57" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -13316,7 +13316,7 @@
       </c>
       <c r="K58" s="84"/>
       <c r="L58" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -13352,7 +13352,7 @@
       </c>
       <c r="K59" s="84"/>
       <c r="L59" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -13626,7 +13626,7 @@
         <v>739</v>
       </c>
       <c r="L20" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="75" r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -13664,7 +13664,7 @@
         <v>737</v>
       </c>
       <c r="L21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="60" r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -13702,7 +13702,7 @@
         <v>375</v>
       </c>
       <c r="L22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="30" r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -13774,7 +13774,7 @@
       </c>
       <c r="K24" s="102"/>
       <c r="L24" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="60" r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -13810,7 +13810,7 @@
       </c>
       <c r="K25" s="103"/>
       <c r="L25" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="30" r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -13846,7 +13846,7 @@
       </c>
       <c r="K26" s="103"/>
       <c r="L26" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -13882,7 +13882,7 @@
       </c>
       <c r="K27" s="103"/>
       <c r="L27" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -13918,7 +13918,7 @@
       </c>
       <c r="K28" s="103"/>
       <c r="L28" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -13954,7 +13954,7 @@
       </c>
       <c r="K29" s="103"/>
       <c r="L29" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -13990,7 +13990,7 @@
       </c>
       <c r="K30" s="103"/>
       <c r="L30" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="75" r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -14026,7 +14026,7 @@
       </c>
       <c r="K31" s="103"/>
       <c r="L31" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -14062,7 +14062,7 @@
       </c>
       <c r="K32" s="103"/>
       <c r="L32" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="75" r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -14098,7 +14098,7 @@
       </c>
       <c r="K33" s="103"/>
       <c r="L33" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -14134,7 +14134,7 @@
       </c>
       <c r="K34" s="103"/>
       <c r="L34" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -14170,7 +14170,7 @@
       </c>
       <c r="K35" s="103"/>
       <c r="L35" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -14206,7 +14206,7 @@
       </c>
       <c r="K36" s="103"/>
       <c r="L36" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="45" r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -14242,7 +14242,7 @@
       </c>
       <c r="K37" s="103"/>
       <c r="L37" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="30" r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -14278,7 +14278,7 @@
       </c>
       <c r="K38" s="103"/>
       <c r="L38" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row ht="30" r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -14314,7 +14314,7 @@
       </c>
       <c r="K39" s="103"/>
       <c r="L39" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>